<commit_message>
MTP036 done and COP rows sent
</commit_message>
<xml_diff>
--- a/observations/orbit_plans/mtp036/nomad_mtp036_plan_generic.xlsx
+++ b/observations/orbit_plans/mtp036/nomad_mtp036_plan_generic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\orbit_plans\mtp036\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A775C34E-500D-442F-81D0-74E01CFD7EA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C19654-94AD-4A34-9707-1BEC6D473581}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10950" yWindow="-14730" windowWidth="18090" windowHeight="12465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1814" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="520">
   <si>
     <t>#orbitType</t>
   </si>
@@ -1223,9 +1223,6 @@
   </si>
   <si>
     <t>2021 JAN 16 12:01:08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:PAVONIS MONS; </t>
   </si>
   <si>
     <t>2021 JAN 16 13:59:03</t>
@@ -1960,8 +1957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="D249" sqref="D249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7137,19 +7134,13 @@
     </row>
     <row r="256" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A256">
-        <v>3</v>
-      </c>
-      <c r="H256" t="s">
-        <v>21</v>
-      </c>
-      <c r="I256" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="L256" t="s">
         <v>400</v>
       </c>
       <c r="M256" t="s">
-        <v>401</v>
+        <v>142</v>
       </c>
     </row>
     <row r="257" spans="1:13" x14ac:dyDescent="0.3">
@@ -7157,21 +7148,21 @@
         <v>14</v>
       </c>
       <c r="L257" t="s">
+        <v>401</v>
+      </c>
+      <c r="M257" t="s">
         <v>402</v>
-      </c>
-      <c r="M257" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="258" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>14</v>
       </c>
+      <c r="I258" t="s">
+        <v>8</v>
+      </c>
       <c r="L258" t="s">
-        <v>404</v>
-      </c>
-      <c r="M258" t="s">
-        <v>142</v>
+        <v>403</v>
       </c>
     </row>
     <row r="259" spans="1:13" x14ac:dyDescent="0.3">
@@ -7185,7 +7176,7 @@
         <v>8</v>
       </c>
       <c r="L259" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="M259" t="s">
         <v>59</v>
@@ -7217,10 +7208,10 @@
         <v>8</v>
       </c>
       <c r="L260" t="s">
+        <v>405</v>
+      </c>
+      <c r="M260" t="s">
         <v>406</v>
-      </c>
-      <c r="M260" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="261" spans="1:13" x14ac:dyDescent="0.3">
@@ -7234,7 +7225,7 @@
         <v>8</v>
       </c>
       <c r="L261" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M261" t="s">
         <v>59</v>
@@ -7266,7 +7257,7 @@
         <v>8</v>
       </c>
       <c r="L262" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="M262" t="s">
         <v>59</v>
@@ -7280,10 +7271,10 @@
         <v>8</v>
       </c>
       <c r="L263" t="s">
+        <v>409</v>
+      </c>
+      <c r="M263" t="s">
         <v>410</v>
-      </c>
-      <c r="M263" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="264" spans="1:13" x14ac:dyDescent="0.3">
@@ -7315,7 +7306,7 @@
         <v>8</v>
       </c>
       <c r="L264" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="M264" t="s">
         <v>59</v>
@@ -7347,10 +7338,10 @@
         <v>8</v>
       </c>
       <c r="L265" t="s">
+        <v>412</v>
+      </c>
+      <c r="M265" t="s">
         <v>413</v>
-      </c>
-      <c r="M265" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="266" spans="1:13" x14ac:dyDescent="0.3">
@@ -7361,10 +7352,10 @@
         <v>8</v>
       </c>
       <c r="L266" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M266" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="267" spans="1:13" x14ac:dyDescent="0.3">
@@ -7375,10 +7366,10 @@
         <v>8</v>
       </c>
       <c r="L267" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="M267" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="268" spans="1:13" x14ac:dyDescent="0.3">
@@ -7407,10 +7398,10 @@
         <v>8</v>
       </c>
       <c r="L268" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="M268" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="269" spans="1:13" x14ac:dyDescent="0.3">
@@ -7421,10 +7412,10 @@
         <v>8</v>
       </c>
       <c r="L269" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="M269" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="270" spans="1:13" x14ac:dyDescent="0.3">
@@ -7453,10 +7444,10 @@
         <v>8</v>
       </c>
       <c r="L270" t="s">
+        <v>418</v>
+      </c>
+      <c r="M270" t="s">
         <v>419</v>
-      </c>
-      <c r="M270" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="271" spans="1:13" x14ac:dyDescent="0.3">
@@ -7485,10 +7476,10 @@
         <v>8</v>
       </c>
       <c r="L271" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M271" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="272" spans="1:13" x14ac:dyDescent="0.3">
@@ -7502,10 +7493,10 @@
         <v>8</v>
       </c>
       <c r="L272" t="s">
+        <v>421</v>
+      </c>
+      <c r="M272" t="s">
         <v>422</v>
-      </c>
-      <c r="M272" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="273" spans="1:13" x14ac:dyDescent="0.3">
@@ -7534,10 +7525,10 @@
         <v>8</v>
       </c>
       <c r="L273" t="s">
+        <v>423</v>
+      </c>
+      <c r="M273" t="s">
         <v>424</v>
-      </c>
-      <c r="M273" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="274" spans="1:13" x14ac:dyDescent="0.3">
@@ -7548,10 +7539,10 @@
         <v>8</v>
       </c>
       <c r="L274" t="s">
+        <v>425</v>
+      </c>
+      <c r="M274" t="s">
         <v>426</v>
-      </c>
-      <c r="M274" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="275" spans="1:13" x14ac:dyDescent="0.3">
@@ -7565,7 +7556,7 @@
         <v>8</v>
       </c>
       <c r="L275" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="M275" t="s">
         <v>59</v>
@@ -7597,7 +7588,7 @@
         <v>8</v>
       </c>
       <c r="L276" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="M276" t="s">
         <v>59</v>
@@ -7632,10 +7623,10 @@
         <v>8</v>
       </c>
       <c r="L277" t="s">
+        <v>429</v>
+      </c>
+      <c r="M277" t="s">
         <v>430</v>
-      </c>
-      <c r="M277" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="278" spans="1:13" x14ac:dyDescent="0.3">
@@ -7646,7 +7637,7 @@
         <v>8</v>
       </c>
       <c r="L278" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M278" t="s">
         <v>59</v>
@@ -7663,7 +7654,7 @@
         <v>8</v>
       </c>
       <c r="L279" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M279" t="s">
         <v>59</v>
@@ -7695,10 +7686,10 @@
         <v>8</v>
       </c>
       <c r="L280" t="s">
+        <v>433</v>
+      </c>
+      <c r="M280" t="s">
         <v>434</v>
-      </c>
-      <c r="M280" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="281" spans="1:13" x14ac:dyDescent="0.3">
@@ -7712,7 +7703,7 @@
         <v>103</v>
       </c>
       <c r="L281" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="M281" t="s">
         <v>105</v>
@@ -7726,10 +7717,10 @@
         <v>8</v>
       </c>
       <c r="L282" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="M282" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="283" spans="1:13" x14ac:dyDescent="0.3">
@@ -7743,7 +7734,7 @@
         <v>8</v>
       </c>
       <c r="L283" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="M283" t="s">
         <v>59</v>
@@ -7775,10 +7766,10 @@
         <v>8</v>
       </c>
       <c r="L284" t="s">
+        <v>438</v>
+      </c>
+      <c r="M284" t="s">
         <v>439</v>
-      </c>
-      <c r="M284" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="285" spans="1:13" x14ac:dyDescent="0.3">
@@ -7789,10 +7780,10 @@
         <v>8</v>
       </c>
       <c r="L285" t="s">
+        <v>440</v>
+      </c>
+      <c r="M285" t="s">
         <v>441</v>
-      </c>
-      <c r="M285" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="286" spans="1:13" x14ac:dyDescent="0.3">
@@ -7821,10 +7812,10 @@
         <v>8</v>
       </c>
       <c r="L286" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="M286" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="287" spans="1:13" x14ac:dyDescent="0.3">
@@ -7856,10 +7847,10 @@
         <v>8</v>
       </c>
       <c r="L287" t="s">
+        <v>443</v>
+      </c>
+      <c r="M287" t="s">
         <v>444</v>
-      </c>
-      <c r="M287" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="288" spans="1:13" x14ac:dyDescent="0.3">
@@ -7870,10 +7861,10 @@
         <v>8</v>
       </c>
       <c r="L288" t="s">
+        <v>445</v>
+      </c>
+      <c r="M288" t="s">
         <v>446</v>
-      </c>
-      <c r="M288" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="289" spans="1:13" x14ac:dyDescent="0.3">
@@ -7884,10 +7875,10 @@
         <v>8</v>
       </c>
       <c r="L289" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="M289" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="290" spans="1:13" x14ac:dyDescent="0.3">
@@ -7919,10 +7910,10 @@
         <v>8</v>
       </c>
       <c r="L290" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="M290" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="291" spans="1:13" x14ac:dyDescent="0.3">
@@ -7933,10 +7924,10 @@
         <v>8</v>
       </c>
       <c r="L291" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="M291" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="292" spans="1:13" x14ac:dyDescent="0.3">
@@ -7947,10 +7938,10 @@
         <v>8</v>
       </c>
       <c r="L292" t="s">
+        <v>450</v>
+      </c>
+      <c r="M292" t="s">
         <v>451</v>
-      </c>
-      <c r="M292" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="293" spans="1:13" x14ac:dyDescent="0.3">
@@ -7964,7 +7955,7 @@
         <v>103</v>
       </c>
       <c r="L293" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="M293" t="s">
         <v>105</v>
@@ -7981,10 +7972,10 @@
         <v>8</v>
       </c>
       <c r="L294" t="s">
+        <v>453</v>
+      </c>
+      <c r="M294" t="s">
         <v>454</v>
-      </c>
-      <c r="M294" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="295" spans="1:13" x14ac:dyDescent="0.3">
@@ -8013,10 +8004,10 @@
         <v>8</v>
       </c>
       <c r="L295" t="s">
+        <v>455</v>
+      </c>
+      <c r="M295" t="s">
         <v>456</v>
-      </c>
-      <c r="M295" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="296" spans="1:13" x14ac:dyDescent="0.3">
@@ -8027,7 +8018,7 @@
         <v>8</v>
       </c>
       <c r="L296" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="M296" t="s">
         <v>59</v>
@@ -8062,10 +8053,10 @@
         <v>8</v>
       </c>
       <c r="L297" t="s">
+        <v>458</v>
+      </c>
+      <c r="M297" t="s">
         <v>459</v>
-      </c>
-      <c r="M297" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="298" spans="1:13" x14ac:dyDescent="0.3">
@@ -8094,7 +8085,7 @@
         <v>8</v>
       </c>
       <c r="L298" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="M298" t="s">
         <v>59</v>
@@ -8111,7 +8102,7 @@
         <v>8</v>
       </c>
       <c r="L299" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="M299" t="s">
         <v>59</v>
@@ -8125,7 +8116,7 @@
         <v>8</v>
       </c>
       <c r="L300" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="M300" t="s">
         <v>59</v>
@@ -8157,7 +8148,7 @@
         <v>8</v>
       </c>
       <c r="L301" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="M301" t="s">
         <v>59</v>
@@ -8174,10 +8165,10 @@
         <v>8</v>
       </c>
       <c r="L302" t="s">
+        <v>464</v>
+      </c>
+      <c r="M302" t="s">
         <v>465</v>
-      </c>
-      <c r="M302" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="303" spans="1:13" x14ac:dyDescent="0.3">
@@ -8206,10 +8197,10 @@
         <v>8</v>
       </c>
       <c r="L303" t="s">
+        <v>466</v>
+      </c>
+      <c r="M303" t="s">
         <v>467</v>
-      </c>
-      <c r="M303" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="304" spans="1:13" x14ac:dyDescent="0.3">
@@ -8220,10 +8211,10 @@
         <v>8</v>
       </c>
       <c r="L304" t="s">
+        <v>468</v>
+      </c>
+      <c r="M304" t="s">
         <v>469</v>
-      </c>
-      <c r="M304" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="305" spans="1:13" x14ac:dyDescent="0.3">
@@ -8252,7 +8243,7 @@
         <v>8</v>
       </c>
       <c r="L305" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="M305" t="s">
         <v>346</v>
@@ -8269,10 +8260,10 @@
         <v>8</v>
       </c>
       <c r="L306" t="s">
+        <v>471</v>
+      </c>
+      <c r="M306" t="s">
         <v>472</v>
-      </c>
-      <c r="M306" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="307" spans="1:13" x14ac:dyDescent="0.3">
@@ -8301,10 +8292,10 @@
         <v>8</v>
       </c>
       <c r="L307" t="s">
+        <v>473</v>
+      </c>
+      <c r="M307" t="s">
         <v>474</v>
-      </c>
-      <c r="M307" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="308" spans="1:13" x14ac:dyDescent="0.3">
@@ -8315,10 +8306,10 @@
         <v>8</v>
       </c>
       <c r="L308" t="s">
+        <v>475</v>
+      </c>
+      <c r="M308" t="s">
         <v>476</v>
-      </c>
-      <c r="M308" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="309" spans="1:13" x14ac:dyDescent="0.3">
@@ -8350,7 +8341,7 @@
         <v>8</v>
       </c>
       <c r="L309" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="M309" t="s">
         <v>23</v>
@@ -8382,10 +8373,10 @@
         <v>8</v>
       </c>
       <c r="L310" t="s">
+        <v>478</v>
+      </c>
+      <c r="M310" t="s">
         <v>479</v>
-      </c>
-      <c r="M310" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="311" spans="1:13" x14ac:dyDescent="0.3">
@@ -8396,10 +8387,10 @@
         <v>8</v>
       </c>
       <c r="L311" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="M311" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="312" spans="1:13" x14ac:dyDescent="0.3">
@@ -8428,10 +8419,10 @@
         <v>8</v>
       </c>
       <c r="L312" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="M312" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="313" spans="1:13" x14ac:dyDescent="0.3">
@@ -8442,10 +8433,10 @@
         <v>8</v>
       </c>
       <c r="L313" t="s">
+        <v>482</v>
+      </c>
+      <c r="M313" t="s">
         <v>483</v>
-      </c>
-      <c r="M313" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="314" spans="1:13" x14ac:dyDescent="0.3">
@@ -8474,10 +8465,10 @@
         <v>8</v>
       </c>
       <c r="L314" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="M314" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="315" spans="1:13" x14ac:dyDescent="0.3">
@@ -8491,10 +8482,10 @@
         <v>8</v>
       </c>
       <c r="L315" t="s">
+        <v>485</v>
+      </c>
+      <c r="M315" t="s">
         <v>486</v>
-      </c>
-      <c r="M315" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="316" spans="1:13" x14ac:dyDescent="0.3">
@@ -8505,7 +8496,7 @@
         <v>8</v>
       </c>
       <c r="L316" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="M316" t="s">
         <v>59</v>
@@ -8522,7 +8513,7 @@
         <v>103</v>
       </c>
       <c r="L317" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="M317" t="s">
         <v>105</v>
@@ -8536,10 +8527,10 @@
         <v>8</v>
       </c>
       <c r="L318" t="s">
+        <v>489</v>
+      </c>
+      <c r="M318" t="s">
         <v>490</v>
-      </c>
-      <c r="M318" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="319" spans="1:13" x14ac:dyDescent="0.3">
@@ -8565,16 +8556,16 @@
         <v>6</v>
       </c>
       <c r="H319" t="s">
+        <v>491</v>
+      </c>
+      <c r="I319" t="s">
+        <v>8</v>
+      </c>
+      <c r="L319" t="s">
         <v>492</v>
       </c>
-      <c r="I319" t="s">
-        <v>8</v>
-      </c>
-      <c r="L319" t="s">
+      <c r="M319" t="s">
         <v>493</v>
-      </c>
-      <c r="M319" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="320" spans="1:13" x14ac:dyDescent="0.3">
@@ -8603,7 +8594,7 @@
         <v>8</v>
       </c>
       <c r="L320" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="M320" t="s">
         <v>59</v>
@@ -8617,7 +8608,7 @@
         <v>8</v>
       </c>
       <c r="L321" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="M321" t="s">
         <v>59</v>
@@ -8652,10 +8643,10 @@
         <v>8</v>
       </c>
       <c r="L322" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="M322" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="323" spans="1:13" x14ac:dyDescent="0.3">
@@ -8666,10 +8657,10 @@
         <v>8</v>
       </c>
       <c r="L323" t="s">
+        <v>497</v>
+      </c>
+      <c r="M323" t="s">
         <v>498</v>
-      </c>
-      <c r="M323" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="324" spans="1:13" x14ac:dyDescent="0.3">
@@ -8698,10 +8689,10 @@
         <v>8</v>
       </c>
       <c r="L324" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="M324" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="325" spans="1:13" x14ac:dyDescent="0.3">
@@ -8712,10 +8703,10 @@
         <v>8</v>
       </c>
       <c r="L325" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="M325" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="326" spans="1:13" x14ac:dyDescent="0.3">
@@ -8744,10 +8735,10 @@
         <v>8</v>
       </c>
       <c r="L326" t="s">
+        <v>501</v>
+      </c>
+      <c r="M326" t="s">
         <v>502</v>
-      </c>
-      <c r="M326" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="327" spans="1:13" x14ac:dyDescent="0.3">
@@ -8779,10 +8770,10 @@
         <v>8</v>
       </c>
       <c r="L327" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="M327" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="328" spans="1:13" x14ac:dyDescent="0.3">
@@ -8793,10 +8784,10 @@
         <v>8</v>
       </c>
       <c r="L328" t="s">
+        <v>504</v>
+      </c>
+      <c r="M328" t="s">
         <v>505</v>
-      </c>
-      <c r="M328" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="329" spans="1:13" x14ac:dyDescent="0.3">
@@ -8807,10 +8798,10 @@
         <v>8</v>
       </c>
       <c r="L329" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="M329" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="330" spans="1:13" x14ac:dyDescent="0.3">
@@ -8842,10 +8833,10 @@
         <v>8</v>
       </c>
       <c r="L330" t="s">
+        <v>507</v>
+      </c>
+      <c r="M330" t="s">
         <v>508</v>
-      </c>
-      <c r="M330" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="331" spans="1:13" x14ac:dyDescent="0.3">
@@ -8856,10 +8847,10 @@
         <v>8</v>
       </c>
       <c r="L331" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="M331" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="332" spans="1:13" x14ac:dyDescent="0.3">
@@ -8888,10 +8879,10 @@
         <v>8</v>
       </c>
       <c r="L332" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="M332" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="333" spans="1:13" x14ac:dyDescent="0.3">
@@ -8920,10 +8911,10 @@
         <v>8</v>
       </c>
       <c r="L333" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="M333" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="334" spans="1:13" x14ac:dyDescent="0.3">
@@ -8937,7 +8928,7 @@
         <v>8</v>
       </c>
       <c r="L334" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="M334" t="s">
         <v>23</v>
@@ -8969,7 +8960,7 @@
         <v>8</v>
       </c>
       <c r="L335" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="M335" t="s">
         <v>59</v>
@@ -8983,7 +8974,7 @@
         <v>8</v>
       </c>
       <c r="L336" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="M336" t="s">
         <v>59</v>
@@ -9018,7 +9009,7 @@
         <v>8</v>
       </c>
       <c r="L337" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="M337" t="s">
         <v>59</v>
@@ -9050,7 +9041,7 @@
         <v>8</v>
       </c>
       <c r="L338" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="M338" t="s">
         <v>59</v>
@@ -9067,7 +9058,7 @@
         <v>8</v>
       </c>
       <c r="L339" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="M339" t="s">
         <v>395</v>
@@ -9090,7 +9081,7 @@
         <v>8</v>
       </c>
       <c r="L340" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="M340" t="s">
         <v>59</v>
@@ -9104,7 +9095,7 @@
         <v>8</v>
       </c>
       <c r="L341" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="M341" t="s">
         <v>398</v>

</xml_diff>